<commit_message>
#323: fix unit test. updating list value separator to `|`
</commit_message>
<xml_diff>
--- a/lutra-tabottr/src/test/resources/test1.xlsx
+++ b/lutra-tabottr/src/test/resources/test1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -118,13 +118,13 @@
     <t xml:space="preserve">classes</t>
   </si>
   <si>
-    <t xml:space="preserve">ex:ClassA1 $$ ex:ClassA2 $$ ex:ClassA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ex:ClassB1 $$ ex:ClassB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ex:ClassC1 $$ ex:ClassC2 $$ ex:ClassC3 $$ ex:ClassC4</t>
+    <t xml:space="preserve">ex:ClassA1 | ex:ClassA2 | ex:ClassA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:ClassB1 | ex:ClassB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:ClassC1 | ex:ClassC2 | ex:ClassC3 | ex:ClassC4</t>
   </si>
   <si>
     <t xml:space="preserve">http://candidate.ottr.xyz/rdf/Triple</t>
@@ -276,15 +276,15 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A8:A10 A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,7 +421,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -436,15 +436,15 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="1" sqref="A8:A10 E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,7 +609,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -624,13 +624,13 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A8:A10 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,7 +715,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -730,15 +730,15 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="1" sqref="A8:A10 A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,7 +827,8 @@
       <c r="B9" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="3" t="b">
+      <c r="C9" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -868,7 +869,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>